<commit_message>
Change C1 to C2 as default
</commit_message>
<xml_diff>
--- a/GasBench_run_template.xlsx
+++ b/GasBench_run_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/brda1352_colorado_edu/Documents/Shared/R stuff/gasbench-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{267C2E9C-B0E7-4B12-BB49-0FECEDF30005}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{267C2E9C-B0E7-4B12-BB49-0FECEDF30005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD8BACAD-241D-4997-BFD3-147A442A5A50}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="0" windowWidth="24255" windowHeight="15315" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20655" yWindow="270" windowWidth="20625" windowHeight="15330" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>dis2.std</t>
   </si>
   <si>
-    <t>IAEA-C1</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>CU YULE</t>
+  </si>
+  <si>
+    <t>IAEA-C2</t>
   </si>
 </sst>
 </file>
@@ -779,7 +779,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -818,7 +818,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -827,7 +827,7 @@
         <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -836,7 +836,7 @@
         <v>110</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -850,7 +850,7 @@
         <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -859,12 +859,12 @@
         <v>110</v>
       </c>
       <c r="J3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -873,7 +873,7 @@
         <v>110</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -882,7 +882,7 @@
         <v>110</v>
       </c>
       <c r="J4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -896,7 +896,7 @@
         <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -905,12 +905,12 @@
         <v>110</v>
       </c>
       <c r="J5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -919,7 +919,7 @@
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
@@ -928,12 +928,12 @@
         <v>110</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -942,7 +942,7 @@
         <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -954,12 +954,12 @@
         <v>110</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -968,7 +968,7 @@
         <v>90</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
@@ -980,12 +980,12 @@
         <v>110</v>
       </c>
       <c r="J8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -994,10 +994,10 @@
         <v>110</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -1006,12 +1006,12 @@
         <v>110</v>
       </c>
       <c r="J9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -1020,10 +1020,10 @@
         <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
@@ -1032,12 +1032,12 @@
         <v>110</v>
       </c>
       <c r="J10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -1046,7 +1046,7 @@
         <v>150</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
         <v>10</v>
@@ -1055,12 +1055,12 @@
         <v>110</v>
       </c>
       <c r="J11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1069,7 +1069,7 @@
         <v>200</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
         <v>10</v>
@@ -1078,12 +1078,12 @@
         <v>110</v>
       </c>
       <c r="J12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -1092,7 +1092,7 @@
         <v>110</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" t="s">
         <v>10</v>
@@ -1101,12 +1101,12 @@
         <v>110</v>
       </c>
       <c r="J13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -1115,7 +1115,7 @@
         <v>110</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
         <v>10</v>
@@ -1124,7 +1124,7 @@
         <v>110</v>
       </c>
       <c r="J14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
         <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" t="s">
         <v>10</v>
@@ -1147,7 +1147,7 @@
         <v>110</v>
       </c>
       <c r="J15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1161,7 +1161,7 @@
         <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
@@ -1170,7 +1170,7 @@
         <v>110</v>
       </c>
       <c r="J16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
         <v>110</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>
@@ -1190,7 +1190,7 @@
         <v>110</v>
       </c>
       <c r="J17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
         <v>110</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" t="s">
         <v>10</v>
@@ -1210,7 +1210,7 @@
         <v>110</v>
       </c>
       <c r="J18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
         <v>110</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
@@ -1233,7 +1233,7 @@
         <v>110</v>
       </c>
       <c r="J19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1244,10 +1244,10 @@
         <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G20" t="s">
         <v>6</v>
@@ -1256,7 +1256,7 @@
         <v>110</v>
       </c>
       <c r="J20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1267,10 +1267,10 @@
         <v>110</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="G21" t="s">
         <v>7</v>
@@ -1279,7 +1279,7 @@
         <v>110</v>
       </c>
       <c r="J21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1290,7 +1290,7 @@
         <v>110</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F22" t="s">
         <v>11</v>
@@ -1302,7 +1302,7 @@
         <v>110</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1313,7 +1313,7 @@
         <v>110</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G23" t="s">
         <v>10</v>
@@ -1322,7 +1322,7 @@
         <v>110</v>
       </c>
       <c r="J23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1333,7 +1333,7 @@
         <v>110</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G24" t="s">
         <v>10</v>
@@ -1342,12 +1342,12 @@
         <v>110</v>
       </c>
       <c r="J24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -1356,7 +1356,7 @@
         <v>110</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G25" t="s">
         <v>10</v>
@@ -1365,7 +1365,7 @@
         <v>110</v>
       </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1379,7 +1379,7 @@
         <v>110</v>
       </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G26" t="s">
         <v>10</v>
@@ -1388,12 +1388,12 @@
         <v>110</v>
       </c>
       <c r="J26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -1402,7 +1402,7 @@
         <v>110</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G27" t="s">
         <v>10</v>
@@ -1411,7 +1411,7 @@
         <v>110</v>
       </c>
       <c r="J27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1425,7 +1425,7 @@
         <v>110</v>
       </c>
       <c r="E28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G28" t="s">
         <v>10</v>
@@ -1434,7 +1434,7 @@
         <v>110</v>
       </c>
       <c r="J28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1445,7 +1445,7 @@
         <v>110</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G29" t="s">
         <v>10</v>
@@ -1454,7 +1454,7 @@
         <v>110</v>
       </c>
       <c r="J29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
         <v>110</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G30" t="s">
         <v>10</v>
@@ -1474,7 +1474,7 @@
         <v>110</v>
       </c>
       <c r="J30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
         <v>110</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G31" t="s">
         <v>10</v>
@@ -1494,7 +1494,7 @@
         <v>110</v>
       </c>
       <c r="J31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1505,10 +1505,10 @@
         <v>110</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="G32" t="s">
         <v>7</v>
@@ -1517,7 +1517,7 @@
         <v>110</v>
       </c>
       <c r="J32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1528,10 +1528,10 @@
         <v>110</v>
       </c>
       <c r="E33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G33" t="s">
         <v>6</v>
@@ -1540,7 +1540,7 @@
         <v>110</v>
       </c>
       <c r="J33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1551,7 +1551,7 @@
         <v>110</v>
       </c>
       <c r="E34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F34" t="s">
         <v>11</v>
@@ -1563,7 +1563,7 @@
         <v>110</v>
       </c>
       <c r="J34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1574,7 +1574,7 @@
         <v>110</v>
       </c>
       <c r="E35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F35" t="s">
         <v>5</v>
@@ -1586,7 +1586,7 @@
         <v>110</v>
       </c>
       <c r="J35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1597,12 +1597,12 @@
         <v>110</v>
       </c>
       <c r="E36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -1611,7 +1611,7 @@
         <v>110</v>
       </c>
       <c r="E37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1639,12 +1639,12 @@
         <v>110</v>
       </c>
       <c r="E39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -1653,7 +1653,7 @@
         <v>110</v>
       </c>
       <c r="E40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1664,7 +1664,7 @@
         <v>110</v>
       </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
         <v>110</v>
       </c>
       <c r="E42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1686,7 +1686,7 @@
         <v>110</v>
       </c>
       <c r="E43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -1697,7 +1697,7 @@
         <v>110</v>
       </c>
       <c r="E44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -1708,7 +1708,7 @@
         <v>110</v>
       </c>
       <c r="E45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -1719,7 +1719,7 @@
         <v>110</v>
       </c>
       <c r="E46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -1730,7 +1730,7 @@
         <v>110</v>
       </c>
       <c r="E47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -1741,12 +1741,12 @@
         <v>110</v>
       </c>
       <c r="E48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
         <v>6</v>
@@ -1755,12 +1755,12 @@
         <v>110</v>
       </c>
       <c r="E49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
@@ -1769,7 +1769,7 @@
         <v>110</v>
       </c>
       <c r="E50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1783,7 +1783,7 @@
         <v>110</v>
       </c>
       <c r="E51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1797,7 +1797,7 @@
         <v>110</v>
       </c>
       <c r="E52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
         <v>110</v>
       </c>
       <c r="E53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1819,7 +1819,7 @@
         <v>110</v>
       </c>
       <c r="E54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1830,7 +1830,7 @@
         <v>110</v>
       </c>
       <c r="E55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>